<commit_message>
add middleware for admin check
</commit_message>
<xml_diff>
--- a/doc/features.xlsx
+++ b/doc/features.xlsx
@@ -118,8 +118,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,8 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,14 +462,15 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.375" customWidth="1"/>
-    <col min="7" max="7" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="6.375" customWidth="1"/>
+    <col min="6" max="6" width="11.375" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -475,16 +485,19 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -644,6 +657,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>